<commit_message>
Avance 03/04/2025_newactualizacion del bot de spam, posibles mejoras
</commit_message>
<xml_diff>
--- a/auto_wsp/logistics/Contactos_enviados.xlsx
+++ b/auto_wsp/logistics/Contactos_enviados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UPG-UNAC\Desktop\NEW_AUTOWSP\logistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UPG-UNAC\Desktop\NEW_AUTOWSP\auto_wsp\logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1044A2CC-7941-461F-B385-372D932E004A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCDBE68-2086-4B60-BBAC-E1317BD3FAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4473B8B1-9492-45E9-ACC4-2D1E3F6019AF}"/>
+    <workbookView xWindow="5820" yWindow="1575" windowWidth="16440" windowHeight="14370" xr2:uid="{4473B8B1-9492-45E9-ACC4-2D1E3F6019AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nombre</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Revision</t>
+  </si>
+  <si>
+    <t>Facultad</t>
   </si>
 </sst>
 </file>
@@ -437,20 +440,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374A4ACF-C083-4D06-A5EA-C5168998FF3F}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,18 +467,21 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>